<commit_message>
Updates time-weighted return formulas to what I think they should be
</commit_message>
<xml_diff>
--- a/outputs/market.xlsx
+++ b/outputs/market.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6821"/>
+  <dimension ref="A1:B6850"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68578,6 +68578,296 @@
         <v>296.26</v>
       </c>
     </row>
+    <row r="6822">
+      <c r="A6822" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-02</t>
+        </is>
+      </c>
+      <c r="B6822" t="n">
+        <v>309.09</v>
+      </c>
+    </row>
+    <row r="6823">
+      <c r="A6823" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-03</t>
+        </is>
+      </c>
+      <c r="B6823" t="n">
+        <v>300.24</v>
+      </c>
+    </row>
+    <row r="6824">
+      <c r="A6824" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-04</t>
+        </is>
+      </c>
+      <c r="B6824" t="n">
+        <v>312.86</v>
+      </c>
+    </row>
+    <row r="6825">
+      <c r="A6825" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-05</t>
+        </is>
+      </c>
+      <c r="B6825" t="n">
+        <v>302.46</v>
+      </c>
+    </row>
+    <row r="6826">
+      <c r="A6826" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-06</t>
+        </is>
+      </c>
+      <c r="B6826" t="n">
+        <v>297.46</v>
+      </c>
+    </row>
+    <row r="6827">
+      <c r="A6827" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-09</t>
+        </is>
+      </c>
+      <c r="B6827" t="n">
+        <v>274.23</v>
+      </c>
+    </row>
+    <row r="6828">
+      <c r="A6828" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-10</t>
+        </is>
+      </c>
+      <c r="B6828" t="n">
+        <v>288.42</v>
+      </c>
+    </row>
+    <row r="6829">
+      <c r="A6829" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-11</t>
+        </is>
+      </c>
+      <c r="B6829" t="n">
+        <v>274.36</v>
+      </c>
+    </row>
+    <row r="6830">
+      <c r="A6830" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-12</t>
+        </is>
+      </c>
+      <c r="B6830" t="n">
+        <v>248.11</v>
+      </c>
+    </row>
+    <row r="6831">
+      <c r="A6831" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-13</t>
+        </is>
+      </c>
+      <c r="B6831" t="n">
+        <v>269.32</v>
+      </c>
+    </row>
+    <row r="6832">
+      <c r="A6832" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-16</t>
+        </is>
+      </c>
+      <c r="B6832" t="n">
+        <v>239.85</v>
+      </c>
+    </row>
+    <row r="6833">
+      <c r="A6833" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-17</t>
+        </is>
+      </c>
+      <c r="B6833" t="n">
+        <v>252.8</v>
+      </c>
+    </row>
+    <row r="6834">
+      <c r="A6834" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-18</t>
+        </is>
+      </c>
+      <c r="B6834" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6835">
+      <c r="A6835" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-19</t>
+        </is>
+      </c>
+      <c r="B6835" t="n">
+        <v>240.51</v>
+      </c>
+    </row>
+    <row r="6836">
+      <c r="A6836" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-20</t>
+        </is>
+      </c>
+      <c r="B6836" t="n">
+        <v>228.8</v>
+      </c>
+    </row>
+    <row r="6837">
+      <c r="A6837" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-23</t>
+        </is>
+      </c>
+      <c r="B6837" t="n">
+        <v>222.95</v>
+      </c>
+    </row>
+    <row r="6838">
+      <c r="A6838" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-24</t>
+        </is>
+      </c>
+      <c r="B6838" t="n">
+        <v>243.15</v>
+      </c>
+    </row>
+    <row r="6839">
+      <c r="A6839" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-25</t>
+        </is>
+      </c>
+      <c r="B6839" t="n">
+        <v>246.79</v>
+      </c>
+    </row>
+    <row r="6840">
+      <c r="A6840" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-26</t>
+        </is>
+      </c>
+      <c r="B6840" t="n">
+        <v>261.2</v>
+      </c>
+    </row>
+    <row r="6841">
+      <c r="A6841" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-27</t>
+        </is>
+      </c>
+      <c r="B6841" t="n">
+        <v>253.42</v>
+      </c>
+    </row>
+    <row r="6842">
+      <c r="A6842" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-30</t>
+        </is>
+      </c>
+      <c r="B6842" t="n">
+        <v>261.65</v>
+      </c>
+    </row>
+    <row r="6843">
+      <c r="A6843" s="1" t="inlineStr">
+        <is>
+          <t>2020-03-31</t>
+        </is>
+      </c>
+      <c r="B6843" t="n">
+        <v>257.75</v>
+      </c>
+    </row>
+    <row r="6844">
+      <c r="A6844" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-01</t>
+        </is>
+      </c>
+      <c r="B6844" t="n">
+        <v>246.15</v>
+      </c>
+    </row>
+    <row r="6845">
+      <c r="A6845" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-02</t>
+        </is>
+      </c>
+      <c r="B6845" t="n">
+        <v>251.83</v>
+      </c>
+    </row>
+    <row r="6846">
+      <c r="A6846" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-03</t>
+        </is>
+      </c>
+      <c r="B6846" t="n">
+        <v>248.19</v>
+      </c>
+    </row>
+    <row r="6847">
+      <c r="A6847" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-06</t>
+        </is>
+      </c>
+      <c r="B6847" t="n">
+        <v>264.86</v>
+      </c>
+    </row>
+    <row r="6848">
+      <c r="A6848" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-07</t>
+        </is>
+      </c>
+      <c r="B6848" t="n">
+        <v>265.13</v>
+      </c>
+    </row>
+    <row r="6849">
+      <c r="A6849" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-08</t>
+        </is>
+      </c>
+      <c r="B6849" t="n">
+        <v>274.03</v>
+      </c>
+    </row>
+    <row r="6850">
+      <c r="A6850" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-09</t>
+        </is>
+      </c>
+      <c r="B6850" t="n">
+        <v>278.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a new performance function to serve as base for the outperformance stats of the pfolio
</commit_message>
<xml_diff>
--- a/outputs/market.xlsx
+++ b/outputs/market.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6860"/>
+  <dimension ref="A1:B6862"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68968,6 +68968,26 @@
         <v>282.97</v>
       </c>
     </row>
+    <row r="6861">
+      <c r="A6861" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-27</t>
+        </is>
+      </c>
+      <c r="B6861" t="n">
+        <v>287.05</v>
+      </c>
+    </row>
+    <row r="6862">
+      <c r="A6862" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-28</t>
+        </is>
+      </c>
+      <c r="B6862" t="n">
+        <v>285.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Performance function works, but could use tweaking for dynamicism
</commit_message>
<xml_diff>
--- a/outputs/market.xlsx
+++ b/outputs/market.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6862"/>
+  <dimension ref="A1:B6875"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -68988,6 +68988,136 @@
         <v>285.73</v>
       </c>
     </row>
+    <row r="6863">
+      <c r="A6863" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-29</t>
+        </is>
+      </c>
+      <c r="B6863" t="n">
+        <v>293.21</v>
+      </c>
+    </row>
+    <row r="6864">
+      <c r="A6864" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-30</t>
+        </is>
+      </c>
+      <c r="B6864" t="n">
+        <v>290.48</v>
+      </c>
+    </row>
+    <row r="6865">
+      <c r="A6865" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-01</t>
+        </is>
+      </c>
+      <c r="B6865" t="n">
+        <v>282.79</v>
+      </c>
+    </row>
+    <row r="6866">
+      <c r="A6866" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-04</t>
+        </is>
+      </c>
+      <c r="B6866" t="n">
+        <v>283.57</v>
+      </c>
+    </row>
+    <row r="6867">
+      <c r="A6867" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-05</t>
+        </is>
+      </c>
+      <c r="B6867" t="n">
+        <v>286.19</v>
+      </c>
+    </row>
+    <row r="6868">
+      <c r="A6868" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-06</t>
+        </is>
+      </c>
+      <c r="B6868" t="n">
+        <v>284.25</v>
+      </c>
+    </row>
+    <row r="6869">
+      <c r="A6869" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-07</t>
+        </is>
+      </c>
+      <c r="B6869" t="n">
+        <v>287.68</v>
+      </c>
+    </row>
+    <row r="6870">
+      <c r="A6870" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-08</t>
+        </is>
+      </c>
+      <c r="B6870" t="n">
+        <v>292.44</v>
+      </c>
+    </row>
+    <row r="6871">
+      <c r="A6871" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-11</t>
+        </is>
+      </c>
+      <c r="B6871" t="n">
+        <v>292.5</v>
+      </c>
+    </row>
+    <row r="6872">
+      <c r="A6872" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-12</t>
+        </is>
+      </c>
+      <c r="B6872" t="n">
+        <v>286.67</v>
+      </c>
+    </row>
+    <row r="6873">
+      <c r="A6873" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-13</t>
+        </is>
+      </c>
+      <c r="B6873" t="n">
+        <v>281.6</v>
+      </c>
+    </row>
+    <row r="6874">
+      <c r="A6874" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-14</t>
+        </is>
+      </c>
+      <c r="B6874" t="n">
+        <v>284.97</v>
+      </c>
+    </row>
+    <row r="6875">
+      <c r="A6875" s="1" t="inlineStr">
+        <is>
+          <t>2020-05-15</t>
+        </is>
+      </c>
+      <c r="B6875" t="n">
+        <v>286.28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>